<commit_message>
Simple add. Make headers bold.
</commit_message>
<xml_diff>
--- a/data/Exercise1.4.xlsx
+++ b/data/Exercise1.4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE3A7901-F9CD-446E-8216-D555777094EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0CDBAF-C822-4ACE-82BF-6E759E62B55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F382A9D4-5506-464C-9DD6-2BB7995D574D}"/>
   </bookViews>
@@ -87,12 +87,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +464,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -466,28 +474,29 @@
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>